<commit_message>
Program-8 Automatic Birthday wisher completed (how to send email using python)
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\Desktop\Codes\Python-practice-programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94584F5-3DB7-4F02-A2A0-5FF24B288CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F212B8D-0E13-400E-8EB6-A15E530B0EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -411,7 +411,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,7 +489,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1">
-        <v>45528</v>
+        <v>45530</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>

</xml_diff>